<commit_message>
added some new x path
</commit_message>
<xml_diff>
--- a/xPath.xlsx
+++ b/xPath.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>x-path for flipkartr</t>
   </si>
@@ -45,6 +45,39 @@
   </si>
   <si>
     <t>//input[@class="_3704LK"]</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>//a[@class="_1_3w1N"]</t>
+  </si>
+  <si>
+    <t>more</t>
+  </si>
+  <si>
+    <t>//*[@id="container"]/div/div[2]/div[1]/div[2]/div[5]/div/div/div/div</t>
+  </si>
+  <si>
+    <t>explore Plus</t>
+  </si>
+  <si>
+    <t>//a[text()="Explore"]</t>
+  </si>
+  <si>
+    <t>grocery</t>
+  </si>
+  <si>
+    <t>//div[@class="xtXmba"and text()="Grocery"]</t>
+  </si>
+  <si>
+    <t>view all for best electronics</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/div[4]/div[3]/div[1]/div/div[1]/div/div/a-absolute x path</t>
+  </si>
+  <si>
+    <t>//div[3]/div[1]/div/div[1]/div/div/a-relative x path</t>
   </si>
 </sst>
 </file>
@@ -379,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F14" sqref="F14:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,8 +491,154 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="19">
+    <mergeCell ref="A12:E13"/>
+    <mergeCell ref="F12:I13"/>
+    <mergeCell ref="A14:E15"/>
+    <mergeCell ref="F14:I15"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="A10:E11"/>
+    <mergeCell ref="F10:I11"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I8"/>
+    <mergeCell ref="A7:E8"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="G3:K3"/>

</xml_diff>

<commit_message>
added new x path
</commit_message>
<xml_diff>
--- a/xPath.xlsx
+++ b/xPath.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>x-path for flipkartr</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>//a[@class="NcOwTe"]</t>
+  </si>
+  <si>
+    <t>My order</t>
+  </si>
+  <si>
+    <t>//a[@class="_16v3bB" and text()="MY ORDERS"]</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38:I38"/>
+      <selection activeCell="F39" sqref="F39:I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,38 +1011,43 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="A34:E35"/>
-    <mergeCell ref="F34:I35"/>
-    <mergeCell ref="A36:E37"/>
-    <mergeCell ref="F36:I37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="A30:E31"/>
-    <mergeCell ref="F30:I31"/>
-    <mergeCell ref="A32:E33"/>
-    <mergeCell ref="F32:I33"/>
-    <mergeCell ref="A23:E24"/>
-    <mergeCell ref="F23:I24"/>
-    <mergeCell ref="A25:E26"/>
-    <mergeCell ref="F25:I26"/>
-    <mergeCell ref="A27:E28"/>
-    <mergeCell ref="F27:I28"/>
-    <mergeCell ref="F17:I18"/>
-    <mergeCell ref="A17:E18"/>
-    <mergeCell ref="A19:E20"/>
-    <mergeCell ref="F19:I20"/>
-    <mergeCell ref="A21:E22"/>
-    <mergeCell ref="F21:I22"/>
-    <mergeCell ref="A12:E13"/>
-    <mergeCell ref="F12:I13"/>
-    <mergeCell ref="A14:E15"/>
-    <mergeCell ref="F14:I15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="F16:I16"/>
+  <mergeCells count="47">
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A39:E40"/>
+    <mergeCell ref="F39:I40"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:J4"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="A10:E11"/>
@@ -1045,13 +1056,36 @@
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F7:I8"/>
     <mergeCell ref="A7:E8"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A12:E13"/>
+    <mergeCell ref="F12:I13"/>
+    <mergeCell ref="A14:E15"/>
+    <mergeCell ref="F14:I15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I18"/>
+    <mergeCell ref="A17:E18"/>
+    <mergeCell ref="A19:E20"/>
+    <mergeCell ref="F19:I20"/>
+    <mergeCell ref="A21:E22"/>
+    <mergeCell ref="F21:I22"/>
+    <mergeCell ref="A23:E24"/>
+    <mergeCell ref="F23:I24"/>
+    <mergeCell ref="A25:E26"/>
+    <mergeCell ref="F25:I26"/>
+    <mergeCell ref="A27:E28"/>
+    <mergeCell ref="F27:I28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="A30:E31"/>
+    <mergeCell ref="F30:I31"/>
+    <mergeCell ref="A32:E33"/>
+    <mergeCell ref="F32:I33"/>
+    <mergeCell ref="A34:E35"/>
+    <mergeCell ref="F34:I35"/>
+    <mergeCell ref="A36:E37"/>
+    <mergeCell ref="F36:I37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="F38:I38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
writing x-path for orangeHRM
</commit_message>
<xml_diff>
--- a/xPath.xlsx
+++ b/xPath.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t>x-path for flipkartr</t>
   </si>
@@ -261,13 +261,19 @@
   </si>
   <si>
     <t>//div[@class="aCgX3e"]</t>
+  </si>
+  <si>
+    <t>x-path for orangeHRM</t>
+  </si>
+  <si>
+    <t>x-path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +284,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -304,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,6 +336,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1582,42 +1610,114 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="81">
-    <mergeCell ref="A71:E72"/>
-    <mergeCell ref="F71:I72"/>
-    <mergeCell ref="A73:E74"/>
-    <mergeCell ref="F73:I74"/>
-    <mergeCell ref="A65:E66"/>
-    <mergeCell ref="F65:I66"/>
-    <mergeCell ref="A67:E68"/>
-    <mergeCell ref="F67:I68"/>
-    <mergeCell ref="A69:E70"/>
-    <mergeCell ref="F69:I70"/>
-    <mergeCell ref="A59:E60"/>
-    <mergeCell ref="F59:I60"/>
-    <mergeCell ref="A61:E62"/>
-    <mergeCell ref="F61:I62"/>
-    <mergeCell ref="A63:E64"/>
-    <mergeCell ref="F63:I64"/>
-    <mergeCell ref="A53:E54"/>
-    <mergeCell ref="F53:I54"/>
-    <mergeCell ref="A55:E56"/>
-    <mergeCell ref="F55:I56"/>
-    <mergeCell ref="A57:E58"/>
-    <mergeCell ref="F57:I58"/>
-    <mergeCell ref="A47:E48"/>
-    <mergeCell ref="F47:I48"/>
-    <mergeCell ref="A49:E50"/>
-    <mergeCell ref="F49:I50"/>
-    <mergeCell ref="A51:E52"/>
-    <mergeCell ref="F51:I52"/>
-    <mergeCell ref="A41:E42"/>
-    <mergeCell ref="F41:I42"/>
-    <mergeCell ref="A43:E44"/>
-    <mergeCell ref="F43:I44"/>
-    <mergeCell ref="A45:E46"/>
-    <mergeCell ref="F45:I46"/>
+  <mergeCells count="84">
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="A75:I78"/>
+    <mergeCell ref="A79:D80"/>
+    <mergeCell ref="E79:I80"/>
+    <mergeCell ref="A32:E33"/>
+    <mergeCell ref="F32:I33"/>
+    <mergeCell ref="A34:E35"/>
+    <mergeCell ref="F34:I35"/>
+    <mergeCell ref="A36:E37"/>
+    <mergeCell ref="F36:I37"/>
+    <mergeCell ref="A27:E28"/>
+    <mergeCell ref="F27:I28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="A30:E31"/>
+    <mergeCell ref="F30:I31"/>
+    <mergeCell ref="A21:E22"/>
+    <mergeCell ref="F21:I22"/>
+    <mergeCell ref="A23:E24"/>
+    <mergeCell ref="F23:I24"/>
+    <mergeCell ref="A25:E26"/>
+    <mergeCell ref="F25:I26"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I18"/>
+    <mergeCell ref="A17:E18"/>
+    <mergeCell ref="A19:E20"/>
+    <mergeCell ref="F19:I20"/>
+    <mergeCell ref="A7:E8"/>
+    <mergeCell ref="A12:E13"/>
+    <mergeCell ref="F12:I13"/>
+    <mergeCell ref="A14:E15"/>
+    <mergeCell ref="F14:I15"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="A39:E40"/>
@@ -1634,37 +1734,40 @@
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F7:I8"/>
-    <mergeCell ref="A7:E8"/>
-    <mergeCell ref="A12:E13"/>
-    <mergeCell ref="F12:I13"/>
-    <mergeCell ref="A14:E15"/>
-    <mergeCell ref="F14:I15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I18"/>
-    <mergeCell ref="A17:E18"/>
-    <mergeCell ref="A19:E20"/>
-    <mergeCell ref="F19:I20"/>
-    <mergeCell ref="A21:E22"/>
-    <mergeCell ref="F21:I22"/>
-    <mergeCell ref="A23:E24"/>
-    <mergeCell ref="F23:I24"/>
-    <mergeCell ref="A25:E26"/>
-    <mergeCell ref="F25:I26"/>
-    <mergeCell ref="A27:E28"/>
-    <mergeCell ref="F27:I28"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="A30:E31"/>
-    <mergeCell ref="F30:I31"/>
-    <mergeCell ref="A32:E33"/>
-    <mergeCell ref="F32:I33"/>
-    <mergeCell ref="A34:E35"/>
-    <mergeCell ref="F34:I35"/>
-    <mergeCell ref="A36:E37"/>
-    <mergeCell ref="F36:I37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="A41:E42"/>
+    <mergeCell ref="F41:I42"/>
+    <mergeCell ref="A43:E44"/>
+    <mergeCell ref="F43:I44"/>
+    <mergeCell ref="A45:E46"/>
+    <mergeCell ref="F45:I46"/>
+    <mergeCell ref="A47:E48"/>
+    <mergeCell ref="F47:I48"/>
+    <mergeCell ref="A49:E50"/>
+    <mergeCell ref="F49:I50"/>
+    <mergeCell ref="A51:E52"/>
+    <mergeCell ref="F51:I52"/>
+    <mergeCell ref="A53:E54"/>
+    <mergeCell ref="F53:I54"/>
+    <mergeCell ref="A55:E56"/>
+    <mergeCell ref="F55:I56"/>
+    <mergeCell ref="A57:E58"/>
+    <mergeCell ref="F57:I58"/>
+    <mergeCell ref="A59:E60"/>
+    <mergeCell ref="F59:I60"/>
+    <mergeCell ref="A61:E62"/>
+    <mergeCell ref="F61:I62"/>
+    <mergeCell ref="A63:E64"/>
+    <mergeCell ref="F63:I64"/>
+    <mergeCell ref="A71:E72"/>
+    <mergeCell ref="F71:I72"/>
+    <mergeCell ref="A73:E74"/>
+    <mergeCell ref="F73:I74"/>
+    <mergeCell ref="A65:E66"/>
+    <mergeCell ref="F65:I66"/>
+    <mergeCell ref="A67:E68"/>
+    <mergeCell ref="F67:I68"/>
+    <mergeCell ref="A69:E70"/>
+    <mergeCell ref="F69:I70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added new page x-path
</commit_message>
<xml_diff>
--- a/xPath.xlsx
+++ b/xPath.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
   <si>
     <t>x-path for flipkartr</t>
   </si>
@@ -303,13 +303,46 @@
   </si>
   <si>
     <t>//div[@id="vp-preview"]</t>
+  </si>
+  <si>
+    <t>learn more &gt;</t>
+  </si>
+  <si>
+    <t>//div[@class="link-icon"and @style="background-color: ;"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR adminstraction </t>
+  </si>
+  <si>
+    <t>//img[@class="lazyloaded"and @src="/assets/Uploads/hr-administration.png.webp"]</t>
+  </si>
+  <si>
+    <t>book for free demo</t>
+  </si>
+  <si>
+    <t>your full name</t>
+  </si>
+  <si>
+    <t>//input[@id="Form_getForm_FullName"]</t>
+  </si>
+  <si>
+    <t>business email</t>
+  </si>
+  <si>
+    <t>//input[@id="Form_getForm_Email"and @tabindex="2"]</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>//select[@id="Form_getForm_Country"and @tabindex="3" and@class="dropdown"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +361,14 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -362,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -374,6 +415,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -659,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K92"/>
+  <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91:I92"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103:I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1874,8 +1918,169 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="96">
+  <mergeCells count="107">
+    <mergeCell ref="A99:D100"/>
+    <mergeCell ref="E99:I100"/>
+    <mergeCell ref="A101:D102"/>
+    <mergeCell ref="E101:I102"/>
+    <mergeCell ref="A103:D104"/>
+    <mergeCell ref="E103:I104"/>
+    <mergeCell ref="A93:D94"/>
+    <mergeCell ref="E93:I94"/>
+    <mergeCell ref="A95:D96"/>
+    <mergeCell ref="E95:I96"/>
+    <mergeCell ref="A97:G98"/>
     <mergeCell ref="A87:D88"/>
     <mergeCell ref="E87:I88"/>
     <mergeCell ref="A89:D90"/>

</xml_diff>

<commit_message>
adding some new x-path
</commit_message>
<xml_diff>
--- a/xPath.xlsx
+++ b/xPath.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="114">
   <si>
     <t>x-path for flipkartr</t>
   </si>
@@ -380,6 +380,12 @@
   </si>
   <si>
     <t>//a[@href="home.aspx"]</t>
+  </si>
+  <si>
+    <t>customer login</t>
+  </si>
+  <si>
+    <t>//font[@face="Verdana" and text()="Customer Login"]</t>
   </si>
 </sst>
 </file>
@@ -747,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K117"/>
+  <dimension ref="A1:K119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116:J117"/>
+      <selection activeCell="E118" sqref="E118:J119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2265,8 +2271,38 @@
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
     </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="116">
+  <mergeCells count="118">
+    <mergeCell ref="A118:D119"/>
+    <mergeCell ref="E118:J119"/>
     <mergeCell ref="A111:J113"/>
     <mergeCell ref="A114:D115"/>
     <mergeCell ref="E114:J115"/>

</xml_diff>